<commit_message>
v1.4 Modify content of error message
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_LOGIN.xlsx
+++ b/LH_TESTCASES/LH_TC_LOGIN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t>Preconditions</t>
   </si>
@@ -174,9 +174,6 @@
 Password: Pass@123</t>
   </si>
   <si>
-    <t>An error message “Login failed. Please check your credentials and try again.” should be displayed.</t>
-  </si>
-  <si>
     <t>LH-TC-Login-003</t>
   </si>
   <si>
@@ -260,6 +257,15 @@
   </si>
   <si>
     <t>User is redirected to the registration (sign-up) page</t>
+  </si>
+  <si>
+    <t>An error message "Invalid credentials" should be displayed.</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>Modify content of error message</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,6 +543,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -865,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="G8" zoomScale="89" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="E7" zoomScale="89" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1019,7 +1026,7 @@
         <v>46</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12" t="s">
@@ -1034,22 +1041,22 @@
         <v>32</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>48</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>49</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>47</v>
+      <c r="G11" s="31" t="s">
+        <v>71</v>
       </c>
       <c r="H11" s="24"/>
       <c r="I11" s="24" t="s">
@@ -1064,29 +1071,29 @@
         <v>32</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="G12" s="12" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12" t="s">
         <v>40</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
@@ -1094,22 +1101,22 @@
         <v>33</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>58</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="G13" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="24" t="s">
@@ -1124,22 +1131,22 @@
         <v>32</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>63</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="27" t="s">
-        <v>65</v>
-      </c>
       <c r="G14" s="12" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
@@ -1154,22 +1161,22 @@
         <v>31</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="E15" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="F15" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="G15" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>71</v>
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="24" t="s">
@@ -1219,7 +1226,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,11 +1329,19 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+    <row r="6" spans="1:15" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="18">
+        <v>45773</v>
+      </c>
     </row>
     <row r="7" spans="1:15" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>

</xml_diff>

<commit_message>
v2.3 fixed a mistake
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_LOGIN.xlsx
+++ b/LH_TESTCASES/LH_TC_LOGIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620"/>
+    <workbookView windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_LOGIN" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="115">
   <si>
     <t>Project name</t>
   </si>
@@ -332,6 +332,9 @@
     <t>System displays: "Invalid credentials".</t>
   </si>
   <si>
+    <t>LH-SRS-LOGIN-008</t>
+  </si>
+  <si>
     <t>LH-TC-LOGIN-015</t>
   </si>
   <si>
@@ -405,6 +408,12 @@
   </si>
   <si>
     <t>Executed TCs</t>
+  </si>
+  <si>
+    <t>v2.4</t>
+  </si>
+  <si>
+    <t>Fixed a mistake</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1239,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1353,6 +1362,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1750,8 +1762,8 @@
   <sheetPr/>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21"/>
@@ -2005,7 +2017,7 @@
       <c r="I13" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="48" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2035,7 +2047,7 @@
       <c r="I14" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="48" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2129,7 +2141,7 @@
       <c r="I17" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="48" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2159,7 +2171,7 @@
       <c r="I18" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="47" t="s">
+      <c r="J18" s="48" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2253,12 +2265,12 @@
       <c r="I21" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="47" t="s">
+      <c r="J21" s="48" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="1" ht="47.25" spans="1:10">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="42" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="28" t="s">
@@ -2290,26 +2302,28 @@
       </c>
     </row>
     <row r="23" ht="47.25" spans="1:10">
-      <c r="A23" s="42"/>
-      <c r="B23" s="28" t="s">
+      <c r="A23" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="B23" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="C23" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="45" t="s">
+      <c r="H23" s="47" t="s">
         <v>33</v>
       </c>
       <c r="I23" s="31" t="s">
@@ -2323,7 +2337,7 @@
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A8:I23" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -2333,7 +2347,6 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <conditionalFormatting sqref="J21">
     <cfRule type="containsText" dxfId="0" priority="16" operator="between" text="Fail">
@@ -2390,10 +2403,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2406,16 +2419,16 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="27" spans="1:15">
       <c r="A1" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -2431,13 +2444,13 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="21" spans="1:15">
       <c r="A2" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" s="10">
         <v>45760</v>
@@ -2456,13 +2469,13 @@
     </row>
     <row r="3" s="3" customFormat="1" ht="37.5" spans="1:4">
       <c r="A3" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="10">
         <v>45766</v>
@@ -2470,13 +2483,13 @@
     </row>
     <row r="4" s="3" customFormat="1" ht="37.5" spans="1:4">
       <c r="A4" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D4" s="10">
         <v>45766</v>
@@ -2484,13 +2497,13 @@
     </row>
     <row r="5" s="3" customFormat="1" ht="37.5" spans="1:4">
       <c r="A5" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D5" s="10">
         <v>45768</v>
@@ -2498,13 +2511,13 @@
     </row>
     <row r="6" s="3" customFormat="1" ht="37.5" spans="1:4">
       <c r="A6" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D6" s="10">
         <v>45773</v>
@@ -2512,13 +2525,13 @@
     </row>
     <row r="7" s="4" customFormat="1" ht="57" spans="1:15">
       <c r="A7" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D7" s="10">
         <v>45788</v>
@@ -2537,13 +2550,13 @@
     </row>
     <row r="8" ht="37.5" spans="1:15">
       <c r="A8" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D8" s="10">
         <v>45789</v>
@@ -2562,13 +2575,13 @@
     </row>
     <row r="9" ht="37.5" spans="1:15">
       <c r="A9" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D9" s="10">
         <v>45792</v>
@@ -2587,16 +2600,30 @@
     </row>
     <row r="10" ht="18.75" spans="1:4">
       <c r="A10" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D10" s="10">
         <v>45792</v>
+      </c>
+    </row>
+    <row r="11" ht="18.75" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="10">
+        <v>45793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>